<commit_message>
Removed depth_max_m as a GLM predictor
</commit_message>
<xml_diff>
--- a/glm transformation and predictor inclusion decisions.xlsx
+++ b/glm transformation and predictor inclusion decisions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="47">
   <si>
     <t>Full</t>
   </si>
@@ -140,6 +140,21 @@
   </si>
   <si>
     <t>totp, cond</t>
+  </si>
+  <si>
+    <t>Remove alk, waterfowl, depth</t>
+  </si>
+  <si>
+    <t>Reduced 5</t>
+  </si>
+  <si>
+    <t>cond, latitude, totP, secchi</t>
+  </si>
+  <si>
+    <t>cond, secchi</t>
+  </si>
+  <si>
+    <t>totp, cond, secchi</t>
   </si>
 </sst>
 </file>
@@ -522,10 +537,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,9 +550,10 @@
     <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.625" customWidth="1"/>
     <col min="5" max="6" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>33</v>
       </c>
@@ -553,8 +569,11 @@
       <c r="F1" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -573,8 +592,11 @@
       <c r="F2" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -585,8 +607,9 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -601,8 +624,9 @@
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -621,8 +645,11 @@
       <c r="F5" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -637,8 +664,9 @@
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="4"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -657,8 +685,11 @@
       <c r="F8" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>1</v>
       </c>
@@ -669,8 +700,9 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
@@ -685,8 +717,9 @@
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
@@ -705,8 +738,11 @@
       <c r="F11" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
@@ -721,8 +757,9 @@
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="4"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -741,8 +778,11 @@
       <c r="F14" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
@@ -753,8 +793,9 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
@@ -769,8 +810,9 @@
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
@@ -789,8 +831,11 @@
       <c r="F17" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
@@ -805,8 +850,9 @@
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="4"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>10</v>
       </c>
@@ -825,8 +871,11 @@
       <c r="F20" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>1</v>
       </c>
@@ -837,8 +886,9 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
@@ -853,8 +903,9 @@
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>4</v>
       </c>
@@ -873,8 +924,11 @@
       <c r="F23" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>3</v>
       </c>
@@ -889,6 +943,7 @@
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>